<commit_message>
added quic deny rule
</commit_message>
<xml_diff>
--- a/internet_gateway/panos/set_commands/internet_gateway_gsb.xlsx
+++ b/internet_gateway/panos/set_commands/internet_gateway_gsb.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="196">
   <si>
     <t>Variable Name</t>
   </si>
@@ -336,6 +336,54 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">set rulebase security rules block-quic source any
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic destination any
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic source-user any
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic category any
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic application quic
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic service application-default
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic hip-profiles any
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic action deny
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic description "blocks quic and forces use of standard ssl for web sessions to help capture url values of encrypted sessions"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic tag Gold
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic log-end yes
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic log-setting default
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">set rulebase security rules MSSP-no-unknown-URL-xfer profile-setting group Outbound-unknownURL
 </t>
   </si>
@@ -612,6 +660,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">set rulebase security rules block-quic tag Silver
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">set rulebase security rules MSSP-allow-outbound profile-setting group MSSP-Silver
 </t>
   </si>
@@ -661,6 +713,10 @@
   </si>
   <si>
     <t xml:space="preserve">set rulebase security rules No-log-ntp-syslog-traffic tag Bronze
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set rulebase security rules block-quic tag Bronze
 </t>
   </si>
   <si>
@@ -1231,7 +1287,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A362"/>
+  <dimension ref="A2:A404"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1864,7 +1920,7 @@
     </row>
     <row r="115" spans="1:1">
       <c r="A115">
-        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic  from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
@@ -1924,20 +1980,20 @@
       </c>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>91</v>
+      <c r="A127">
+        <f>SUBSTITUTE("set rulebase security rules block-quic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-no-unknown-URL-xfer to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules block-quic from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-no-unknown-URL-xfer from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A129" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="130" spans="1:1">
@@ -2002,13 +2058,13 @@
     </row>
     <row r="142" spans="1:1">
       <c r="A142">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules MSSP-no-unknown-URL-xfer to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set rulebase security rules MSSP-no-unknown-URL-xfer from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
@@ -2073,20 +2129,20 @@
       </c>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" t="s">
-        <v>116</v>
+      <c r="A156">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A158" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="159" spans="1:1">
@@ -2150,20 +2206,20 @@
       </c>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" t="s">
-        <v>129</v>
+      <c r="A171">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A173" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="174" spans="1:1">
@@ -2227,20 +2283,20 @@
       </c>
     </row>
     <row r="186" spans="1:1">
-      <c r="A186" t="s">
-        <v>142</v>
+      <c r="A186">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:1">
-      <c r="A188">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A188" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="189" spans="1:1">
@@ -2304,832 +2360,1048 @@
       </c>
     </row>
     <row r="201" spans="1:1">
-      <c r="A201" t="s">
-        <v>155</v>
+      <c r="A201">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" t="s">
-        <v>147</v>
+      <c r="A202">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>47</v>
+        <v>156</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="208" spans="1:1">
-      <c r="A208">
-        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A208" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="209" spans="1:1">
-      <c r="A209">
-        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic  from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A209" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>86</v>
+        <v>159</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="221" spans="1:1">
-      <c r="A221">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A221" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:1">
-      <c r="A223" t="s">
-        <v>104</v>
+      <c r="A223">
+        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic  from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" t="s">
-        <v>116</v>
+      <c r="A235">
+        <f>SUBSTITUTE("set rulebase security rules block-quic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules block-quic from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:1">
-      <c r="A237">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A237" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>162</v>
+        <v>102</v>
       </c>
     </row>
     <row r="249" spans="1:1">
-      <c r="A249" t="s">
-        <v>163</v>
+      <c r="A249">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:1">
-      <c r="A250" t="s">
-        <v>129</v>
+      <c r="A250">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A251" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A252" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
     </row>
     <row r="264" spans="1:1">
-      <c r="A264" t="s">
-        <v>165</v>
+      <c r="A264">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:1">
-      <c r="A265" t="s">
-        <v>142</v>
+      <c r="A265">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:1">
-      <c r="A266">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A266" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="267" spans="1:1">
-      <c r="A267">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A267" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
     </row>
     <row r="279" spans="1:1">
-      <c r="A279" t="s">
-        <v>154</v>
+      <c r="A279">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:1">
-      <c r="A280" t="s">
-        <v>155</v>
+      <c r="A280">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>47</v>
+        <v>143</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
     </row>
     <row r="287" spans="1:1">
-      <c r="A287">
-        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A287" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="288" spans="1:1">
-      <c r="A288">
-        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic  from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A288" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>82</v>
+        <v>177</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>83</v>
+        <v>178</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
     </row>
     <row r="294" spans="1:1">
-      <c r="A294" t="s">
-        <v>85</v>
+      <c r="A294">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:1">
-      <c r="A295" t="s">
-        <v>86</v>
+      <c r="A295">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="300" spans="1:1">
-      <c r="A300">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A300" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="301" spans="1:1">
-      <c r="A301">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A301" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <f>SUBSTITUTE("set rulebase security rules No-log-ntp-syslog-traffic  from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="328" spans="1:1">
-      <c r="A328" t="s">
-        <v>176</v>
+      <c r="A328">
+        <f>SUBSTITUTE("set rulebase security rules block-quic to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:1">
-      <c r="A329" t="s">
-        <v>129</v>
+      <c r="A329">
+        <f>SUBSTITUTE("set rulebase security rules block-quic from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:1">
-      <c r="A330">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A330" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="331" spans="1:1">
-      <c r="A331">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A331" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
     </row>
     <row r="342" spans="1:1">
-      <c r="A342" t="s">
-        <v>177</v>
+      <c r="A342">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:1">
-      <c r="A343" t="s">
-        <v>178</v>
+      <c r="A343">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-allow-outbound from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
     </row>
     <row r="345" spans="1:1">
-      <c r="A345">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
-        <v>0</v>
+      <c r="A345" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="346" spans="1:1">
-      <c r="A346">
-        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
-        <v>0</v>
+      <c r="A346" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>180</v>
+        <v>128</v>
       </c>
     </row>
     <row r="357" spans="1:1">
-      <c r="A357" t="s">
-        <v>181</v>
+      <c r="A357">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="358" spans="1:1">
-      <c r="A358" t="s">
-        <v>154</v>
+      <c r="A358">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-SSL-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1">
+      <c r="A363" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1">
+      <c r="A364" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1">
+      <c r="A365" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1">
+      <c r="A366" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1">
+      <c r="A367" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1">
+      <c r="A368" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1">
+      <c r="A370" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1">
+      <c r="A371" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1">
+      <c r="A372">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1">
+      <c r="A373">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-non-def-web-ports from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1">
+      <c r="A374" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1">
+      <c r="A375" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1">
+      <c r="A376" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1">
+      <c r="A377" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1">
+      <c r="A378" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1">
+      <c r="A379" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1">
+      <c r="A380" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1">
+      <c r="A381" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1">
+      <c r="A382" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1">
+      <c r="A383" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1">
+      <c r="A384" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1">
+      <c r="A385" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1">
+      <c r="A386" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1">
+      <c r="A387">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps to {{ ZONE_UNTRUST }}", "{{ ZONE_UNTRUST }}", 'values'!B9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1">
+      <c r="A388">
+        <f>SUBSTITUTE("set rulebase security rules MSSP-find-non-def-apps from {{ ZONE_TRUST }}", "{{ ZONE_TRUST }}", 'values'!B8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1">
+      <c r="A389" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1">
+      <c r="A390" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1">
+      <c r="A391" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1">
+      <c r="A392" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1">
+      <c r="A393" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1">
+      <c r="A394" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1">
+      <c r="A395" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1">
+      <c r="A396" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1">
+      <c r="A397" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1">
+      <c r="A398" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1">
+      <c r="A399" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1">
+      <c r="A400" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1">
+      <c r="A401" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1">
+      <c r="A402" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1">
+      <c r="A403" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1">
+      <c r="A404" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>